<commit_message>
Updated changes as per tap comments
- install ignitors after pix by rocket
</commit_message>
<xml_diff>
--- a/Heisey L3 Checklist 209 11 12.xlsx
+++ b/Heisey L3 Checklist 209 11 12.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Assembly checklist" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>Middle pull switch</t>
   </si>
   <si>
-    <t>Calibrate proton (vertical on pad)</t>
-  </si>
-  <si>
     <t>Install ignitor</t>
   </si>
   <si>
@@ -319,9 +316,6 @@
     <t>Arm NC tracker via Wifi Switch</t>
   </si>
   <si>
-    <t>Check  eveyting a once over</t>
-  </si>
-  <si>
     <t>Arming sequence:</t>
   </si>
   <si>
@@ -341,12 +335,6 @@
   </si>
   <si>
     <t xml:space="preserve">     Eggtimer Tx</t>
-  </si>
-  <si>
-    <t>Log to proton and arm</t>
-  </si>
-  <si>
-    <t>Arm Proton</t>
   </si>
   <si>
     <t>Login onto quanum</t>
@@ -430,9 +418,6 @@
   </si>
   <si>
     <t>Double Check Make sure launch rail is slightly from the crowd and locked.</t>
-  </si>
-  <si>
-    <t>Set up cameras (see separate instructions)</t>
   </si>
   <si>
     <r>
@@ -466,6 +451,21 @@
   </si>
   <si>
     <t>Record values:</t>
+  </si>
+  <si>
+    <t>Set up remote cameras (see separate instructions)</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Check continuity</t>
+  </si>
+  <si>
+    <t>Check  eveything a once over</t>
+  </si>
+  <si>
+    <t>Turn on mobius camera</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -647,11 +647,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -729,6 +738,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -740,16 +753,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <top style="thin">
           <color indexed="64"/>
-        </bottom>
+        </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
+        <bottom style="thin">
           <color indexed="64"/>
-        </top>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -766,11 +779,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:B1048572" totalsRowShown="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
-  <autoFilter ref="A1:B1048572"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C1048548" totalsRowShown="0" headerRowBorderDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="A1:C1048548">
+    <filterColumn colId="2"/>
+  </autoFilter>
+  <tableColumns count="3">
     <tableColumn id="1" name="Check"/>
     <tableColumn id="2" name="Step" dataDxfId="0"/>
+    <tableColumn id="3" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1039,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B131"/>
+  <dimension ref="A1:C129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113:XFD115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1051,96 +1067,99 @@
     <col min="2" max="2" width="73" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="37.5">
+        <v>32</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="37.5">
       <c r="A2" s="1"/>
       <c r="B2" s="21" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="18.75">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18.75">
       <c r="A3" s="1"/>
       <c r="B3" s="21" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1">
       <c r="B4" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1">
       <c r="B5" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1">
       <c r="B6" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B7" s="25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" s="27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B9" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1">
-      <c r="B7" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="B8" s="27" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1">
-      <c r="B9" s="9" t="s">
+    <row r="10" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B10" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1">
-      <c r="B10" s="10" t="s">
+    <row r="11" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B11" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1">
-      <c r="B11" s="9" t="s">
+    <row r="12" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B12" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1">
-      <c r="B12" s="10" t="s">
+    <row r="13" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B13" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B14" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B15" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1">
-      <c r="B13" s="9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1">
-      <c r="B14" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1">
-      <c r="B15" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:3">
       <c r="A16" s="1"/>
       <c r="B16" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1"/>
       <c r="B17" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1158,13 +1177,13 @@
     <row r="20" spans="1:2">
       <c r="A20" s="1"/>
       <c r="B20" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1"/>
       <c r="B21" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1182,7 +1201,7 @@
     <row r="24" spans="1:2">
       <c r="A24" s="1"/>
       <c r="B24" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1194,13 +1213,13 @@
     <row r="26" spans="1:2">
       <c r="A26" s="1"/>
       <c r="B26" s="26" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1"/>
       <c r="B27" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1212,19 +1231,19 @@
     <row r="29" spans="1:2">
       <c r="A29" s="1"/>
       <c r="B29" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1"/>
       <c r="B30" s="11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1"/>
       <c r="B31" s="12" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1248,197 +1267,197 @@
     <row r="35" spans="1:2">
       <c r="A35" s="1"/>
       <c r="B35" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1"/>
       <c r="B36" s="11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1"/>
       <c r="B37" s="11" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1"/>
       <c r="B38" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1"/>
       <c r="B39" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1"/>
       <c r="B40" s="12" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1">
       <c r="A41" s="1"/>
       <c r="B41" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="19.5" thickBot="1">
       <c r="A42" s="18"/>
       <c r="B42" s="22" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="B43" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="B44" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="B45" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="B46" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="B47" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="B48" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="2:2" ht="15.75" thickBot="1">
       <c r="B54" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="2:2" ht="19.5" thickBot="1">
       <c r="B55" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="2:2">
       <c r="B56" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="2:2">
       <c r="B57" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="2:2">
       <c r="B58" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="2:2">
       <c r="B59" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="2:2">
       <c r="B60" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="2:2">
       <c r="B62" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="2:2">
       <c r="B63" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="2:2">
       <c r="B64" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="B65" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="B66" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="B67" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="B68" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="18.75">
       <c r="A69" s="1"/>
       <c r="B69" s="21" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="1"/>
       <c r="B70" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="1"/>
       <c r="B71" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1456,31 +1475,31 @@
     <row r="74" spans="1:2">
       <c r="A74" s="1"/>
       <c r="B74" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="1"/>
       <c r="B75" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="1"/>
       <c r="B76" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="1"/>
       <c r="B77" s="11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="1"/>
       <c r="B78" s="11" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1504,7 +1523,7 @@
     <row r="82" spans="1:2">
       <c r="A82" s="1"/>
       <c r="B82" s="11" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1516,7 +1535,7 @@
     <row r="84" spans="1:2" ht="18.75">
       <c r="A84" s="1"/>
       <c r="B84" s="21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1540,13 +1559,13 @@
     <row r="88" spans="1:2">
       <c r="A88" s="1"/>
       <c r="B88" s="11" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="1"/>
       <c r="B89" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1558,13 +1577,13 @@
     <row r="91" spans="1:2">
       <c r="A91" s="1"/>
       <c r="B91" s="11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="1"/>
       <c r="B92" s="11" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="18.75">
@@ -1576,19 +1595,19 @@
     <row r="94" spans="1:2">
       <c r="A94" s="1"/>
       <c r="B94" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="1"/>
       <c r="B95" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="1"/>
       <c r="B96" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1606,7 +1625,7 @@
     <row r="99" spans="1:2" ht="18.75">
       <c r="A99" s="1"/>
       <c r="B99" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1624,19 +1643,19 @@
     <row r="103" spans="1:2">
       <c r="A103" s="1"/>
       <c r="B103" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="1"/>
       <c r="B104" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="1"/>
       <c r="B105" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1648,7 +1667,7 @@
     <row r="107" spans="1:2">
       <c r="A107" s="1"/>
       <c r="B107" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1660,7 +1679,7 @@
     <row r="109" spans="1:2">
       <c r="A109" s="1"/>
       <c r="B109" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1678,70 +1697,70 @@
     <row r="112" spans="1:2">
       <c r="A112" s="1"/>
       <c r="B112" s="17" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="1"/>
       <c r="B113" s="17" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="1"/>
-      <c r="B114" s="17" t="s">
-        <v>28</v>
+      <c r="B114" s="11" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="1"/>
-      <c r="B115" s="17" t="s">
-        <v>108</v>
+      <c r="B115" s="11" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="1"/>
-      <c r="B116" s="17" t="s">
-        <v>98</v>
+      <c r="B116" s="11" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="1"/>
-      <c r="B117" s="11" t="s">
-        <v>101</v>
+      <c r="B117" s="14" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="1"/>
-      <c r="B118" s="11" t="s">
-        <v>102</v>
+      <c r="B118" s="14" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="1"/>
-      <c r="B119" s="11" t="s">
-        <v>106</v>
+      <c r="B119" s="14" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="1"/>
       <c r="B120" s="14" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="1"/>
-      <c r="B121" s="14" t="s">
-        <v>104</v>
+      <c r="B121" s="16" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="1"/>
       <c r="B122" s="14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="30">
       <c r="A123" s="1"/>
       <c r="B123" s="16" t="s">
         <v>79</v>
@@ -1749,42 +1768,36 @@
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="1"/>
-      <c r="B124" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="30">
+      <c r="B124" s="31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
       <c r="A125" s="1"/>
-      <c r="B125" s="16" t="s">
-        <v>80</v>
+      <c r="B125" s="31" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="1"/>
       <c r="B126" s="24" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="1"/>
       <c r="B127" s="14" t="s">
-        <v>99</v>
+        <v>139</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="1"/>
-      <c r="B128" s="14" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="129" spans="1:2" ht="18.75">
       <c r="A129" s="1"/>
       <c r="B129" s="21" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2">
-      <c r="A131" s="1"/>
+        <v>136</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1799,8 +1812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1811,110 +1824,110 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="B2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="B6" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="B7" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="B9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="B10" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="B11" s="28" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1">
       <c r="B12" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="30">
       <c r="B13" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="B15" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="B16" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="30">
       <c r="B20" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="30">
       <c r="B21" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added color codes to visual check list
</commit_message>
<xml_diff>
--- a/Heisey L3 Checklist 209 11 12.xlsx
+++ b/Heisey L3 Checklist 209 11 12.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11910"/>
   </bookViews>
   <sheets>
     <sheet name="Assembly checklist" sheetId="1" r:id="rId1"/>
     <sheet name="Night before prep" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="145">
   <si>
     <t>Make sure all other nuts are tight</t>
   </si>
@@ -383,9 +383,6 @@
   </si>
   <si>
     <t>Pack CO2 charge cups - one spoon Pyrodex-P/BP mixture (5 parts P, 1 part BP)</t>
-  </si>
-  <si>
-    <t>Verify resistence of 7 igniters is 0.8-1.3 ohms</t>
   </si>
   <si>
     <t>Align NC with payload  tube</t>
@@ -456,9 +453,6 @@
     <t>Set up remote cameras (see separate instructions)</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>Check continuity</t>
   </si>
   <si>
@@ -466,13 +460,31 @@
   </si>
   <si>
     <t>Turn on mobius camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  3 - 12 in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1 - 15 in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  4 - full</t>
+  </si>
+  <si>
+    <t>Cut 8 ignitors and color code both ends</t>
+  </si>
+  <si>
+    <t>Prepare two ignitors in dual charge cup</t>
+  </si>
+  <si>
+    <t>Verify resistence of 8 igniters is 0.8-1.3 ohms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,6 +554,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -563,7 +582,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -647,20 +666,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -739,9 +749,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -749,7 +765,7 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -779,14 +795,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C1048548" totalsRowShown="0" headerRowBorderDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="A1:C1048548">
-    <filterColumn colId="2"/>
-  </autoFilter>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:B135" totalsRowShown="0" headerRowBorderDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="A1:B135"/>
+  <tableColumns count="2">
     <tableColumn id="1" name="Check"/>
     <tableColumn id="2" name="Step" dataDxfId="0"/>
-    <tableColumn id="3" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1047,756 +1060,783 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C129"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113:XFD115"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="73" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>33</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="30" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="37.5">
+    </row>
+    <row r="2" spans="1:2" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75">
+    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="21" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B4" s="8" t="s">
+    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="32"/>
+      <c r="B8" s="33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B5" s="9" t="s">
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="9" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B6" s="10" t="s">
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B7" s="25" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" s="27" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B9" s="9" t="s">
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="27" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B10" s="10" t="s">
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B11" s="9" t="s">
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B12" s="10" t="s">
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B13" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B14" s="9" t="s">
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B15" s="8" t="s">
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="26" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="B26" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="11" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="B31" s="26" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="B36" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A41" s="1"/>
-      <c r="B41" s="12" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A42" s="18"/>
-      <c r="B42" s="22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="B43" s="7" t="s">
+    <row r="47" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="18"/>
+      <c r="B47" s="22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="B44" s="7" t="s">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="B45" s="7" t="s">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="B46" s="7" t="s">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="B47" s="7" t="s">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="B48" s="7" t="s">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="7" t="s">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="2:2">
-      <c r="B50" s="7" t="s">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="7" t="s">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="52" spans="2:2">
-      <c r="B52" s="7" t="s">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="2:2">
-      <c r="B53" s="7" t="s">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="15.75" thickBot="1">
-      <c r="B54" s="7" t="s">
+    <row r="59" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="19.5" thickBot="1">
-      <c r="B55" s="22" t="s">
+    <row r="60" spans="2:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="2:2">
-      <c r="B56" s="7" t="s">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="2:2">
-      <c r="B57" s="7" t="s">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="2:2">
-      <c r="B58" s="7" t="s">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="2:2">
-      <c r="B59" s="7" t="s">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="2:2">
-      <c r="B60" s="7" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="2:2">
-      <c r="B61" s="7" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="2:2">
-      <c r="B62" s="7" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="2:2">
-      <c r="B63" s="7" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="2:2">
-      <c r="B64" s="7" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="B65" s="7" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="B66" s="7" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="B67" s="7" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
-      <c r="B68" s="7" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="18.75">
-      <c r="A69" s="1"/>
-      <c r="B69" s="21" t="s">
+    <row r="74" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A74" s="1"/>
+      <c r="B74" s="21" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="1"/>
-      <c r="B70" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="1"/>
-      <c r="B71" s="11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="1"/>
-      <c r="B72" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="1"/>
-      <c r="B73" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="1"/>
-      <c r="B74" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="18.75">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
-      <c r="B84" s="21" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="B84" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
-      <c r="B89" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
+      <c r="B89" s="21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="11" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="18.75">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
-      <c r="B93" s="21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
+      <c r="B93" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
-      <c r="B94" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
+      <c r="B94" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
-      <c r="B95" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
+      <c r="B95" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
-      <c r="B98" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="18.75">
+      <c r="B98" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
-      <c r="B99" s="23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
+      <c r="B99" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
-      <c r="B100" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
+      <c r="B100" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="1"/>
+      <c r="B101" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
-      <c r="B103" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
+      <c r="B103" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
-      <c r="B104" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
+      <c r="B104" s="23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
-      <c r="B105" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
-      <c r="A106" s="1"/>
-      <c r="B106" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2">
+      <c r="B105" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="1"/>
+      <c r="B108" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1"/>
+      <c r="B109" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="1"/>
+      <c r="B110" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="1"/>
+      <c r="B111" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1"/>
+      <c r="B112" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
-      <c r="A108" s="1"/>
-      <c r="B108" s="11" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="1"/>
+      <c r="B113" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
-      <c r="A109" s="1"/>
-      <c r="B109" s="14" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1"/>
+      <c r="B114" s="14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
-      <c r="A110" s="1"/>
-      <c r="B110" s="17" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1"/>
+      <c r="B115" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
-      <c r="A111" s="1"/>
-      <c r="B111" s="17" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="1"/>
+      <c r="B116" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
-      <c r="A112" s="1"/>
-      <c r="B112" s="17" t="s">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="1"/>
+      <c r="B117" s="17" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
-      <c r="A113" s="1"/>
-      <c r="B113" s="17" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="1"/>
+      <c r="B118" s="17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
-      <c r="A114" s="1"/>
-      <c r="B114" s="11" t="s">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="1"/>
+      <c r="B119" s="11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
-      <c r="A115" s="1"/>
-      <c r="B115" s="11" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="1"/>
+      <c r="B120" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
-      <c r="A116" s="1"/>
-      <c r="B116" s="11" t="s">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="1"/>
+      <c r="B121" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
-      <c r="A117" s="1"/>
-      <c r="B117" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2">
-      <c r="A118" s="1"/>
-      <c r="B118" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2">
-      <c r="A119" s="1"/>
-      <c r="B119" s="14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2">
-      <c r="A120" s="1"/>
-      <c r="B120" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2">
-      <c r="A121" s="1"/>
-      <c r="B121" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="14" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
-      <c r="B123" s="16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2">
+      <c r="B123" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
-      <c r="B124" s="31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2">
+      <c r="B124" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
-      <c r="B125" s="31" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2">
+      <c r="B125" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
-      <c r="B126" s="24" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2">
+      <c r="B126" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
-    </row>
-    <row r="129" spans="1:2" ht="18.75">
+      <c r="B128" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
-      <c r="B129" s="21" t="s">
+      <c r="B129" s="30" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="1"/>
+      <c r="B130" s="30" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="1"/>
+      <c r="B131" s="24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="1"/>
+      <c r="B132" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="1"/>
+    </row>
+    <row r="134" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A134" s="1"/>
+      <c r="B134" s="21" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1809,20 +1849,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="49.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -1830,102 +1870,102 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="28" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="30">
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="30">
+    <row r="20" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="30">
+    <row r="21" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>50</v>
       </c>

</xml_diff>